<commit_message>
work in progress before merge
</commit_message>
<xml_diff>
--- a/FileStorage/ExcelFiles/excelinsomnia.xlsx
+++ b/FileStorage/ExcelFiles/excelinsomnia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\birle\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDA1B24-C2A8-4104-A2AC-272DD6B094BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6969ABE4-39AA-445C-94E4-D74347442A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>DormitoryName</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>45 Forest Rd</t>
+  </si>
+  <si>
+    <t>DormitoryAmount</t>
   </si>
 </sst>
 </file>
@@ -400,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -411,7 +414,7 @@
     <col min="1" max="1" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,13 +422,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -433,13 +439,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="2">
+        <v>200</v>
+      </c>
+      <c r="D2" s="2">
         <v>101</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -447,13 +456,16 @@
         <v>4</v>
       </c>
       <c r="C3" s="2">
+        <v>200</v>
+      </c>
+      <c r="D3" s="2">
         <v>102</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -461,13 +473,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="2">
+        <v>200</v>
+      </c>
+      <c r="D4" s="2">
         <v>103</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -475,13 +490,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
+        <v>300</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -489,9 +507,12 @@
         <v>7</v>
       </c>
       <c r="C6" s="2">
+        <v>300</v>
+      </c>
+      <c r="D6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>